<commit_message>
Updated ITA model - 2025-08-06 12:19
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SuppXLS/Scen_advanced_features.xlsx
+++ b/VerveStacks_ITA/SuppXLS/Scen_advanced_features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BEBA60-1221-4328-A5F4-305001227557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1B8BBA-9FA0-4608-9904-2A92EA38D7BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="1" xr2:uid="{22AE2797-EE70-457C-AC96-4BB7B6BD4E04}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="2" xr2:uid="{22AE2797-EE70-457C-AC96-4BB7B6BD4E04}"/>
   </bookViews>
   <sheets>
     <sheet name="veda input" sheetId="1" r:id="rId1"/>
@@ -3246,9 +3246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F77616-F3F2-4CAD-9718-D78F2778A52A}">
   <dimension ref="B2:S17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -4117,1177 +4115,1175 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA60F42B-F2D1-44E2-B5F0-15531EB389CB}">
-  <dimension ref="A1:AW25"/>
+  <dimension ref="B2:AX26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.86328125" customWidth="1"/>
-    <col min="7" max="7" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.46484375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="6" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.53125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="6" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="3" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="6" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="6" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6" bestFit="1" customWidth="1"/>
-    <col min="45" max="46" width="4" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="49" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.86328125" customWidth="1"/>
+    <col min="8" max="8" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="6" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="3" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="6" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="4" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="6" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="4" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="16" t="s">
+    <row r="2" spans="2:50" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:49" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
+    <row r="3" spans="2:50" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B3" t="s">
         <v>203</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>204</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>205</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E3" t="s">
         <v>206</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F3" t="s">
         <v>207</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G3" t="s">
         <v>208</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H3" t="s">
         <v>209</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I3" t="s">
         <v>210</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J3" t="s">
         <v>211</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
         <v>39</v>
       </c>
-      <c r="L2">
+      <c r="M3">
         <v>40</v>
       </c>
-      <c r="M2">
+      <c r="N3">
         <v>41</v>
       </c>
-      <c r="N2">
+      <c r="O3">
         <v>79</v>
       </c>
-      <c r="O2">
+      <c r="P3">
         <v>80</v>
       </c>
-      <c r="P2">
+      <c r="Q3">
         <v>81</v>
       </c>
-      <c r="Q2">
+      <c r="R3">
         <v>119</v>
       </c>
-      <c r="R2">
+      <c r="S3">
         <v>120</v>
       </c>
-      <c r="S2">
+      <c r="T3">
         <v>121</v>
       </c>
-      <c r="T2">
+      <c r="U3">
         <v>159</v>
       </c>
-      <c r="U2">
+      <c r="V3">
         <v>160</v>
       </c>
-      <c r="V2">
+      <c r="W3">
         <v>161</v>
       </c>
-      <c r="W2">
+      <c r="X3">
         <v>199</v>
       </c>
-      <c r="X2">
+      <c r="Y3">
         <v>200</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="AD2" s="3">
-        <f t="shared" ref="AD2:AR3" si="0">J2</f>
-        <v>1</v>
-      </c>
-      <c r="AE2" s="3">
+      <c r="AE3" s="3">
+        <f t="shared" ref="AE3:AS4" si="0">K3</f>
+        <v>1</v>
+      </c>
+      <c r="AF3" s="3">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="AF2" s="3">
+      <c r="AG3" s="3">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="AG2" s="3">
+      <c r="AH3" s="3">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="AH2" s="3">
+      <c r="AI3" s="3">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
-      <c r="AI2" s="3">
+      <c r="AJ3" s="3">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="AJ2" s="3">
+      <c r="AK3" s="3">
         <f t="shared" si="0"/>
         <v>81</v>
       </c>
-      <c r="AK2" s="3">
+      <c r="AL3" s="3">
         <f t="shared" si="0"/>
         <v>119</v>
       </c>
-      <c r="AL2" s="3">
+      <c r="AM3" s="3">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="AM2" s="3">
+      <c r="AN3" s="3">
         <f t="shared" si="0"/>
         <v>121</v>
       </c>
-      <c r="AN2" s="3">
+      <c r="AO3" s="3">
         <f t="shared" si="0"/>
         <v>159</v>
       </c>
-      <c r="AO2" s="3">
+      <c r="AP3" s="3">
         <f t="shared" si="0"/>
         <v>160</v>
       </c>
-      <c r="AP2" s="3">
+      <c r="AQ3" s="3">
         <f t="shared" si="0"/>
         <v>161</v>
       </c>
-      <c r="AQ2" s="3">
+      <c r="AR3" s="3">
         <f t="shared" si="0"/>
         <v>199</v>
       </c>
-      <c r="AR2" s="3">
+      <c r="AS3" s="3">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="4" spans="2:50" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
         <v>213</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>214</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>215</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E4" t="s">
         <v>215</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F4" t="s">
         <v>216</v>
       </c>
-      <c r="F3" s="17">
+      <c r="G4" s="17">
         <v>39.18</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="H4" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="H3" s="17">
+      <c r="I4" s="17">
         <v>43.5</v>
       </c>
-      <c r="I3">
+      <c r="J4">
         <v>81</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
         <v>1.1100000000000001</v>
       </c>
-      <c r="L3">
+      <c r="M4">
         <v>6.18</v>
       </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
         <v>1.1100000000000001</v>
       </c>
-      <c r="O3">
+      <c r="P4">
         <v>6.18</v>
       </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
         <v>1.1100000000000001</v>
       </c>
-      <c r="R3">
+      <c r="S4">
         <v>6.18</v>
       </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
         <v>1.1100000000000001</v>
       </c>
-      <c r="U3">
+      <c r="V4">
         <v>6.18</v>
       </c>
-      <c r="V3">
-        <v>1</v>
-      </c>
-      <c r="W3">
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
         <v>1.1100000000000001</v>
       </c>
-      <c r="X3">
+      <c r="Y4">
         <v>6.18</v>
       </c>
-      <c r="AC3">
-        <f t="shared" ref="AC3:AR4" si="1">I3</f>
+      <c r="AD4">
+        <f t="shared" ref="AD4:AS5" si="1">J4</f>
         <v>81</v>
       </c>
-      <c r="AD3">
+      <c r="AE4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AE3">
+      <c r="AF4">
         <f t="shared" si="0"/>
         <v>1.1100000000000001</v>
       </c>
-      <c r="AF3">
+      <c r="AG4">
         <f t="shared" si="0"/>
         <v>6.18</v>
       </c>
-      <c r="AG3">
+      <c r="AH4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AH3">
+      <c r="AI4">
         <f t="shared" si="0"/>
         <v>1.1100000000000001</v>
       </c>
-      <c r="AI3">
+      <c r="AJ4">
         <f t="shared" si="0"/>
         <v>6.18</v>
       </c>
-      <c r="AJ3">
+      <c r="AK4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AK3">
+      <c r="AL4">
         <f t="shared" si="0"/>
         <v>1.1100000000000001</v>
       </c>
-      <c r="AL3">
+      <c r="AM4">
         <f t="shared" si="0"/>
         <v>6.18</v>
       </c>
-      <c r="AM3">
+      <c r="AN4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AN3">
+      <c r="AO4">
         <f t="shared" si="0"/>
         <v>1.1100000000000001</v>
       </c>
-      <c r="AO3">
+      <c r="AP4">
         <f t="shared" si="0"/>
         <v>6.18</v>
       </c>
-      <c r="AP3">
+      <c r="AQ4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AQ3">
+      <c r="AR4">
         <f t="shared" si="0"/>
         <v>1.1100000000000001</v>
       </c>
-      <c r="AR3">
+      <c r="AS4">
         <f t="shared" si="0"/>
         <v>6.18</v>
       </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="5" spans="2:50" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
         <v>218</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>215</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
         <v>219</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E5" t="s">
         <v>215</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F5" t="s">
         <v>216</v>
       </c>
-      <c r="F4" s="17">
+      <c r="G5" s="17">
         <v>19.34</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="H5" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="H4" s="17">
+      <c r="I5" s="17">
         <v>28.67</v>
       </c>
-      <c r="I4">
+      <c r="J5">
         <v>82</v>
       </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
         <v>1.48</v>
       </c>
-      <c r="L4">
+      <c r="M5">
         <v>10</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
         <v>1.48</v>
       </c>
-      <c r="O4">
+      <c r="P5">
         <v>10</v>
       </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4">
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
         <v>1.48</v>
       </c>
-      <c r="R4">
+      <c r="S5">
         <v>10</v>
       </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-      <c r="T4">
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
         <v>1.48</v>
       </c>
-      <c r="U4">
+      <c r="V5">
         <v>10</v>
       </c>
-      <c r="V4">
-        <v>1</v>
-      </c>
-      <c r="W4">
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
         <v>1.48</v>
       </c>
-      <c r="X4">
+      <c r="Y5">
         <v>10</v>
       </c>
-      <c r="AC4">
+      <c r="AD5">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="AD4">
+      <c r="AE5">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AE4">
+      <c r="AF5">
         <f t="shared" si="1"/>
         <v>1.48</v>
       </c>
-      <c r="AF4">
+      <c r="AG5">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="AG4">
+      <c r="AH5">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AH4">
+      <c r="AI5">
         <f t="shared" si="1"/>
         <v>1.48</v>
       </c>
-      <c r="AI4">
+      <c r="AJ5">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="AJ4">
+      <c r="AK5">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AK4">
+      <c r="AL5">
         <f t="shared" si="1"/>
         <v>1.48</v>
       </c>
-      <c r="AL4">
+      <c r="AM5">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="AM4">
+      <c r="AN5">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AN4">
+      <c r="AO5">
         <f t="shared" si="1"/>
         <v>1.48</v>
       </c>
-      <c r="AO4">
+      <c r="AP5">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="AP4">
+      <c r="AQ5">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AQ4">
+      <c r="AR5">
         <f t="shared" si="1"/>
         <v>1.48</v>
       </c>
-      <c r="AR4">
+      <c r="AS5">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:49" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="AC6" s="2" t="s">
+    <row r="7" spans="2:50" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="AD7" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:49" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" t="s">
+    <row r="8" spans="2:50" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B8" t="s">
         <v>203</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
         <v>204</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D8" t="s">
         <v>205</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E8" t="s">
         <v>206</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F8" t="s">
         <v>207</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G8" t="s">
         <v>208</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H8" t="s">
         <v>211</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
         <v>29</v>
       </c>
-      <c r="J7">
+      <c r="K8">
         <v>30</v>
       </c>
-      <c r="K7">
+      <c r="L8">
         <v>31</v>
       </c>
-      <c r="L7">
+      <c r="M8">
         <v>59</v>
       </c>
-      <c r="M7">
+      <c r="N8">
         <v>60</v>
       </c>
-      <c r="N7">
+      <c r="O8">
         <v>61</v>
       </c>
-      <c r="O7">
+      <c r="P8">
         <v>89</v>
       </c>
-      <c r="P7">
+      <c r="Q8">
         <v>90</v>
       </c>
-      <c r="Q7">
+      <c r="R8">
         <v>91</v>
       </c>
-      <c r="R7">
+      <c r="S8">
         <v>119</v>
       </c>
-      <c r="S7">
+      <c r="T8">
         <v>120</v>
       </c>
-      <c r="T7">
+      <c r="U8">
         <v>121</v>
       </c>
-      <c r="U7">
+      <c r="V8">
         <v>149</v>
       </c>
-      <c r="V7">
+      <c r="W8">
         <v>150</v>
       </c>
-      <c r="W7">
+      <c r="X8">
         <v>151</v>
       </c>
-      <c r="X7">
+      <c r="Y8">
         <v>179</v>
       </c>
-      <c r="Y7">
+      <c r="Z8">
         <v>180</v>
       </c>
-      <c r="Z7">
+      <c r="AA8">
         <v>181</v>
       </c>
-      <c r="AA7">
+      <c r="AB8">
         <v>200</v>
       </c>
-      <c r="AC7" s="3" t="s">
+      <c r="AD8" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="AD7" s="3">
-        <f t="shared" ref="AD7:AS9" si="2">H7</f>
-        <v>1</v>
-      </c>
-      <c r="AE7" s="3">
+      <c r="AE8" s="3">
+        <f t="shared" ref="AE8:AT10" si="2">I8</f>
+        <v>1</v>
+      </c>
+      <c r="AF8" s="3">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="AF7" s="3">
+      <c r="AG8" s="3">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="AG7" s="3">
+      <c r="AH8" s="3">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="AH7" s="3">
+      <c r="AI8" s="3">
         <f t="shared" si="2"/>
         <v>59</v>
       </c>
-      <c r="AI7" s="3">
+      <c r="AJ8" s="3">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="AJ7" s="3">
+      <c r="AK8" s="3">
         <f t="shared" si="2"/>
         <v>61</v>
       </c>
-      <c r="AK7" s="3">
+      <c r="AL8" s="3">
         <f t="shared" si="2"/>
         <v>89</v>
       </c>
-      <c r="AL7" s="3">
+      <c r="AM8" s="3">
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
-      <c r="AM7" s="3">
+      <c r="AN8" s="3">
         <f t="shared" si="2"/>
         <v>91</v>
       </c>
-      <c r="AN7" s="3">
+      <c r="AO8" s="3">
         <f t="shared" si="2"/>
         <v>119</v>
       </c>
-      <c r="AO7" s="3">
+      <c r="AP8" s="3">
         <f t="shared" si="2"/>
         <v>120</v>
       </c>
-      <c r="AP7" s="3">
+      <c r="AQ8" s="3">
         <f t="shared" si="2"/>
         <v>121</v>
       </c>
-      <c r="AQ7" s="3">
+      <c r="AR8" s="3">
         <f t="shared" si="2"/>
         <v>149</v>
       </c>
-      <c r="AR7" s="3">
+      <c r="AS8" s="3">
         <f t="shared" si="2"/>
         <v>150</v>
       </c>
-      <c r="AS7" s="3">
+      <c r="AT8" s="3">
         <f t="shared" si="2"/>
         <v>151</v>
       </c>
-      <c r="AT7" s="3">
-        <f t="shared" ref="AN7:AW9" si="3">X7</f>
+      <c r="AU8" s="3">
+        <f t="shared" ref="AO8:AX10" si="3">Y8</f>
         <v>179</v>
       </c>
-      <c r="AU7" s="3">
+      <c r="AV8" s="3">
         <f t="shared" si="3"/>
         <v>180</v>
       </c>
-      <c r="AV7" s="3">
+      <c r="AW8" s="3">
         <f t="shared" si="3"/>
         <v>181</v>
       </c>
-      <c r="AW7" s="3">
+      <c r="AX8" s="3">
         <f t="shared" si="3"/>
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="9" spans="2:50" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
         <v>220</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C9" t="s">
         <v>215</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D9" t="s">
         <v>215</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E9" t="s">
         <v>215</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F9" t="s">
         <v>221</v>
       </c>
-      <c r="F8" s="17">
+      <c r="G9" s="17">
         <v>30.18</v>
       </c>
-      <c r="G8">
+      <c r="H9">
         <v>83</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
         <v>3.72</v>
       </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8">
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
         <v>3.72</v>
       </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="P8">
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
         <v>3.72</v>
       </c>
-      <c r="Q8">
-        <v>1</v>
-      </c>
-      <c r="R8">
-        <v>1</v>
-      </c>
-      <c r="S8">
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
         <v>3.72</v>
       </c>
-      <c r="T8">
-        <v>1</v>
-      </c>
-      <c r="U8">
-        <v>1</v>
-      </c>
-      <c r="V8">
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9">
+        <v>1</v>
+      </c>
+      <c r="W9">
         <v>3.72</v>
       </c>
-      <c r="W8">
-        <v>1</v>
-      </c>
-      <c r="X8">
-        <v>1</v>
-      </c>
-      <c r="Y8">
+      <c r="X9">
+        <v>1</v>
+      </c>
+      <c r="Y9">
+        <v>1</v>
+      </c>
+      <c r="Z9">
         <v>3.72</v>
       </c>
-      <c r="Z8">
-        <v>1</v>
-      </c>
-      <c r="AA8">
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AB9">
         <v>3.72</v>
       </c>
-      <c r="AC8">
-        <f t="shared" ref="AC8:AC9" si="4">G8</f>
+      <c r="AD9">
+        <f t="shared" ref="AD9:AD10" si="4">H9</f>
         <v>83</v>
       </c>
-      <c r="AD8">
+      <c r="AE9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AE8">
+      <c r="AF9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AF8">
+      <c r="AG9">
         <f t="shared" si="2"/>
         <v>3.72</v>
       </c>
-      <c r="AG8">
+      <c r="AH9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AH8">
+      <c r="AI9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AI8">
+      <c r="AJ9">
         <f t="shared" si="2"/>
         <v>3.72</v>
       </c>
-      <c r="AJ8">
+      <c r="AK9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AK8">
+      <c r="AL9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AL8">
+      <c r="AM9">
         <f t="shared" si="2"/>
         <v>3.72</v>
       </c>
-      <c r="AM8">
+      <c r="AN9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AN8">
+      <c r="AO9">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AO8">
+      <c r="AP9">
         <f t="shared" si="3"/>
         <v>3.72</v>
       </c>
-      <c r="AP8">
+      <c r="AQ9">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AQ8">
+      <c r="AR9">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AR8">
+      <c r="AS9">
         <f t="shared" si="3"/>
         <v>3.72</v>
       </c>
-      <c r="AS8">
+      <c r="AT9">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AT8">
+      <c r="AU9">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AU8">
+      <c r="AV9">
         <f t="shared" si="3"/>
         <v>3.72</v>
       </c>
-      <c r="AV8">
+      <c r="AW9">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AW8">
+      <c r="AX9">
         <f t="shared" si="3"/>
         <v>3.72</v>
       </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="10" spans="2:50" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
         <v>222</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C10" t="s">
         <v>215</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D10" t="s">
         <v>215</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E10" t="s">
         <v>215</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F10" t="s">
         <v>221</v>
       </c>
-      <c r="F9" s="17">
+      <c r="G10" s="17">
         <v>19.73</v>
       </c>
-      <c r="G9">
+      <c r="H10">
         <v>84</v>
       </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
         <v>13.27</v>
       </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9">
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
         <v>13.27</v>
       </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="P9">
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
         <v>13.27</v>
       </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-      <c r="S9">
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
         <v>13.27</v>
       </c>
-      <c r="T9">
-        <v>1</v>
-      </c>
-      <c r="U9">
-        <v>1</v>
-      </c>
-      <c r="V9">
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+      <c r="W10">
         <v>13.27</v>
       </c>
-      <c r="W9">
-        <v>1</v>
-      </c>
-      <c r="X9">
-        <v>1</v>
-      </c>
-      <c r="Y9">
+      <c r="X10">
+        <v>1</v>
+      </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="Z10">
         <v>13.27</v>
       </c>
-      <c r="Z9">
-        <v>1</v>
-      </c>
-      <c r="AA9">
+      <c r="AA10">
+        <v>1</v>
+      </c>
+      <c r="AB10">
         <v>13.27</v>
       </c>
-      <c r="AC9">
+      <c r="AD10">
         <f t="shared" si="4"/>
         <v>84</v>
       </c>
-      <c r="AD9">
+      <c r="AE10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AE9">
+      <c r="AF10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AF9">
+      <c r="AG10">
         <f t="shared" si="2"/>
         <v>13.27</v>
       </c>
-      <c r="AG9">
+      <c r="AH10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AH9">
+      <c r="AI10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AI9">
+      <c r="AJ10">
         <f t="shared" si="2"/>
         <v>13.27</v>
       </c>
-      <c r="AJ9">
+      <c r="AK10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AK9">
+      <c r="AL10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AL9">
+      <c r="AM10">
         <f t="shared" si="2"/>
         <v>13.27</v>
       </c>
-      <c r="AM9">
+      <c r="AN10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AN9">
+      <c r="AO10">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AO9">
+      <c r="AP10">
         <f t="shared" si="3"/>
         <v>13.27</v>
       </c>
-      <c r="AP9">
+      <c r="AQ10">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AQ9">
+      <c r="AR10">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AR9">
+      <c r="AS10">
         <f t="shared" si="3"/>
         <v>13.27</v>
       </c>
-      <c r="AS9">
+      <c r="AT10">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AT9">
+      <c r="AU10">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AU9">
+      <c r="AV10">
         <f t="shared" si="3"/>
         <v>13.27</v>
       </c>
-      <c r="AV9">
+      <c r="AW10">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AW9">
+      <c r="AX10">
         <f t="shared" si="3"/>
         <v>13.27</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.45">
-      <c r="A12" s="16" t="s">
+    <row r="13" spans="2:50" x14ac:dyDescent="0.45">
+      <c r="B13" s="16" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.45">
-      <c r="A13" s="18" t="s">
+    <row r="14" spans="2:50" x14ac:dyDescent="0.45">
+      <c r="B14" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-    </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.45">
-      <c r="A14" s="18" t="s">
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+    </row>
+    <row r="15" spans="2:50" x14ac:dyDescent="0.45">
+      <c r="B15" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-    </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.45">
-      <c r="A15" s="18" t="s">
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+    </row>
+    <row r="16" spans="2:50" x14ac:dyDescent="0.45">
+      <c r="B16" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A17" s="18" t="s">
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B18" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="C18" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="D18" s="18" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A18" s="18" t="s">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B19" s="18" t="s">
         <v>230</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="C19" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="C18" s="18">
+      <c r="D19" s="18">
         <v>253</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="18" t="s">
+    <row r="20" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="C20" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="C19" s="18">
+      <c r="D20" s="18">
         <v>203</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="18" t="s">
+    <row r="21" spans="2:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B21" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="C21" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="C20" s="18">
+      <c r="D21" s="18">
         <v>82</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="H21" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="I21" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="J21" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="J20" s="3">
+      <c r="K21" s="3">
         <v>2019</v>
       </c>
-      <c r="K20" s="3">
+      <c r="L21" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A21" s="18" t="s">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B22" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="C22" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="C21" s="18">
+      <c r="D22" s="18">
         <v>242</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H22" t="s">
         <v>240</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I22" t="s">
         <v>246</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J22" t="s">
         <v>247</v>
       </c>
-      <c r="J21">
-        <f>AC3</f>
+      <c r="K22">
+        <f>AD4</f>
         <v>81</v>
       </c>
-      <c r="K21">
+      <c r="L22">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A22" s="18" t="s">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B23" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="C23" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="C22" s="18">
+      <c r="D23" s="18">
         <v>226</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H23" t="s">
         <v>240</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I23" t="s">
         <v>80</v>
       </c>
-      <c r="J22">
-        <f>AC4</f>
+      <c r="K23">
+        <f>AD5</f>
         <v>82</v>
       </c>
-      <c r="K22">
+      <c r="L23">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A23" s="18" t="s">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B24" s="18" t="s">
         <v>242</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="C24" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="C23" s="18">
+      <c r="D24" s="18">
         <v>174</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H24" t="s">
         <v>240</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I24" t="s">
         <v>22</v>
       </c>
-      <c r="J23">
-        <f>AC8</f>
+      <c r="K24">
+        <f>AD9</f>
         <v>83</v>
       </c>
-      <c r="K23">
+      <c r="L24">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A24" s="18" t="s">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B25" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="C25" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="C24" s="18">
+      <c r="D25" s="18">
         <v>258</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H25" t="s">
         <v>240</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I25" t="s">
         <v>15</v>
       </c>
-      <c r="J24">
-        <f>AC9</f>
+      <c r="K25">
+        <f>AD10</f>
         <v>84</v>
       </c>
-      <c r="K24">
+      <c r="L25">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A25" s="18" t="s">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B26" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="C26" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="C25" s="18">
+      <c r="D26" s="18">
         <v>135</v>
       </c>
     </row>
@@ -5299,660 +5295,660 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B99335-61C3-404F-89AE-B281012B672E}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="B2:K46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
         <v>71</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="C2">
+      <c r="D3">
         <v>25</v>
       </c>
-      <c r="D2">
+      <c r="E3">
         <v>0.5</v>
       </c>
-      <c r="E2">
+      <c r="F3">
         <v>0.5</v>
       </c>
-      <c r="F2">
+      <c r="G3">
         <v>120</v>
       </c>
-      <c r="G2">
+      <c r="H3">
         <v>120</v>
       </c>
-      <c r="H2">
+      <c r="I3">
         <v>0.5</v>
       </c>
-      <c r="I2">
+      <c r="J3">
         <v>10</v>
       </c>
-      <c r="J2">
+      <c r="K3">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="C3">
+      <c r="D4">
         <v>30</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <v>100</v>
       </c>
-      <c r="G3">
+      <c r="H4">
         <v>100</v>
       </c>
-      <c r="H3">
+      <c r="I4">
         <v>0.75</v>
       </c>
-      <c r="I3">
+      <c r="J4">
         <v>15</v>
       </c>
-      <c r="J3">
+      <c r="K4">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="C4">
+      <c r="D5">
         <v>35</v>
       </c>
-      <c r="D4">
+      <c r="E5">
         <v>1.5</v>
       </c>
-      <c r="E4">
+      <c r="F5">
         <v>1.5</v>
       </c>
-      <c r="F4">
+      <c r="G5">
         <v>80</v>
       </c>
-      <c r="G4">
+      <c r="H5">
         <v>80</v>
       </c>
-      <c r="H4">
+      <c r="I5">
         <v>1.25</v>
       </c>
-      <c r="I4">
+      <c r="J5">
         <v>20</v>
       </c>
-      <c r="J4">
+      <c r="K5">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="C5">
+      <c r="D6">
         <v>50</v>
       </c>
-      <c r="D5">
+      <c r="E6">
         <v>2</v>
       </c>
-      <c r="E5">
+      <c r="F6">
         <v>2</v>
       </c>
-      <c r="F5">
+      <c r="G6">
         <v>60</v>
       </c>
-      <c r="G5">
+      <c r="H6">
         <v>60</v>
       </c>
-      <c r="H5">
+      <c r="I6">
         <v>1.75</v>
       </c>
-      <c r="I5">
+      <c r="J6">
         <v>25</v>
       </c>
-      <c r="J5">
+      <c r="K6">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="C6">
+      <c r="D7">
         <v>55</v>
       </c>
-      <c r="D6">
+      <c r="E7">
         <v>4</v>
       </c>
-      <c r="E6">
+      <c r="F7">
         <v>4</v>
       </c>
-      <c r="F6">
+      <c r="G7">
         <v>45</v>
       </c>
-      <c r="G6">
+      <c r="H7">
         <v>45</v>
       </c>
-      <c r="H6">
+      <c r="I7">
         <v>3</v>
       </c>
-      <c r="I6">
+      <c r="J7">
         <v>40</v>
       </c>
-      <c r="J6">
+      <c r="K7">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
         <v>26</v>
       </c>
-      <c r="C7">
+      <c r="D8">
         <v>35</v>
       </c>
-      <c r="D7">
+      <c r="E8">
         <v>3</v>
       </c>
-      <c r="E7">
+      <c r="F8">
         <v>3</v>
       </c>
-      <c r="F7">
+      <c r="G8">
         <v>40</v>
       </c>
-      <c r="G7">
+      <c r="H8">
         <v>40</v>
       </c>
-      <c r="H7">
+      <c r="I8">
         <v>2</v>
       </c>
-      <c r="I7">
+      <c r="J8">
         <v>25</v>
       </c>
-      <c r="J7">
+      <c r="K8">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="C8">
+      <c r="D9">
         <v>40</v>
       </c>
-      <c r="D8">
+      <c r="E9">
         <v>5</v>
       </c>
-      <c r="E8">
+      <c r="F9">
         <v>5</v>
       </c>
-      <c r="F8">
+      <c r="G9">
         <v>30</v>
       </c>
-      <c r="G8">
+      <c r="H9">
         <v>30</v>
       </c>
-      <c r="H8">
+      <c r="I9">
         <v>3</v>
       </c>
-      <c r="I8">
+      <c r="J9">
         <v>35</v>
       </c>
-      <c r="J8">
+      <c r="K9">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C10" t="s">
         <v>27</v>
       </c>
-      <c r="C9">
+      <c r="D10">
         <v>30</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
         <v>120</v>
       </c>
-      <c r="G9">
+      <c r="H10">
         <v>120</v>
       </c>
-      <c r="H9">
+      <c r="I10">
         <v>0.4</v>
       </c>
-      <c r="I9">
+      <c r="J10">
         <v>10</v>
       </c>
-      <c r="J9">
+      <c r="K10">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C11" t="s">
         <v>73</v>
       </c>
-      <c r="C10">
+      <c r="D11">
         <v>35</v>
       </c>
-      <c r="D10">
+      <c r="E11">
         <v>2</v>
       </c>
-      <c r="E10">
+      <c r="F11">
         <v>2</v>
       </c>
-      <c r="F10">
+      <c r="G11">
         <v>60</v>
       </c>
-      <c r="G10">
+      <c r="H11">
         <v>60</v>
       </c>
-      <c r="H10">
+      <c r="I11">
         <v>1.5</v>
       </c>
-      <c r="I10">
+      <c r="J11">
         <v>20</v>
       </c>
-      <c r="J10">
+      <c r="K11">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="C11">
+      <c r="D12">
         <v>38</v>
       </c>
-      <c r="D11">
+      <c r="E12">
         <v>5</v>
       </c>
-      <c r="E11">
+      <c r="F12">
         <v>5</v>
       </c>
-      <c r="F11">
+      <c r="G12">
         <v>30</v>
       </c>
-      <c r="G11">
+      <c r="H12">
         <v>30</v>
       </c>
-      <c r="H11">
+      <c r="I12">
         <v>5</v>
       </c>
-      <c r="I11">
+      <c r="J12">
         <v>40</v>
       </c>
-      <c r="J11">
+      <c r="K12">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C13" t="s">
         <v>24</v>
       </c>
-      <c r="C12">
+      <c r="D13">
         <v>42</v>
       </c>
-      <c r="D12">
+      <c r="E13">
         <v>7</v>
       </c>
-      <c r="E12">
+      <c r="F13">
         <v>7</v>
       </c>
-      <c r="F12">
+      <c r="G13">
         <v>20</v>
       </c>
-      <c r="G12">
+      <c r="H13">
         <v>20</v>
       </c>
-      <c r="H12">
+      <c r="I13">
         <v>8</v>
       </c>
-      <c r="I12">
+      <c r="J13">
         <v>60</v>
       </c>
-      <c r="J12">
+      <c r="K13">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C14" t="s">
         <v>28</v>
       </c>
-      <c r="C13">
+      <c r="D14">
         <v>45</v>
       </c>
-      <c r="D13">
+      <c r="E14">
         <v>6</v>
       </c>
-      <c r="E13">
+      <c r="F14">
         <v>6</v>
       </c>
-      <c r="F13">
+      <c r="G14">
         <v>25</v>
       </c>
-      <c r="G13">
+      <c r="H14">
         <v>25</v>
       </c>
-      <c r="H13">
+      <c r="I14">
         <v>6</v>
       </c>
-      <c r="I13">
+      <c r="J14">
         <v>50</v>
       </c>
-      <c r="J13">
+      <c r="K14">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C15" t="s">
         <v>29</v>
       </c>
-      <c r="C14">
+      <c r="D15">
         <v>48</v>
       </c>
-      <c r="D14">
+      <c r="E15">
         <v>8</v>
       </c>
-      <c r="E14">
+      <c r="F15">
         <v>8</v>
       </c>
-      <c r="F14">
+      <c r="G15">
         <v>15</v>
       </c>
-      <c r="G14">
+      <c r="H15">
         <v>15</v>
       </c>
-      <c r="H14">
+      <c r="I15">
         <v>9</v>
       </c>
-      <c r="I14">
+      <c r="J15">
         <v>70</v>
       </c>
-      <c r="J14">
+      <c r="K15">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C16" t="s">
         <v>30</v>
       </c>
-      <c r="C15">
+      <c r="D16">
         <v>70</v>
       </c>
-      <c r="D15">
+      <c r="E16">
         <v>24</v>
       </c>
-      <c r="E15">
+      <c r="F16">
         <v>24</v>
       </c>
-      <c r="F15">
+      <c r="G16">
         <v>5</v>
       </c>
-      <c r="G15">
+      <c r="H16">
         <v>5</v>
       </c>
-      <c r="H15">
+      <c r="I16">
         <v>48</v>
       </c>
-      <c r="I15">
+      <c r="J16">
         <v>100</v>
       </c>
-      <c r="J15">
+      <c r="K16">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="A19" s="5" t="s">
+    <row r="20" spans="2:4" ht="17.649999999999999" x14ac:dyDescent="0.45">
+      <c r="B20" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" s="6" t="s">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B22" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" s="7" t="s">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B23" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" s="7" t="s">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B24" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" s="7" t="s">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B25" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" s="7" t="s">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B26" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A26" s="7" t="s">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B27" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" s="7" t="s">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B28" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A28" s="7" t="s">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B29" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A29" s="7" t="s">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B30" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A30" s="8"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A31" s="8" t="s">
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B31" s="8"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B32" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A32" s="8"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A33" s="8" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B33" s="8"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B34" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A34" s="8"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A35" s="8" t="s">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B35" s="8"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B36" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="17.649999999999999" x14ac:dyDescent="0.45">
-      <c r="A39" s="5" t="s">
+    <row r="40" spans="2:2" ht="17.649999999999999" x14ac:dyDescent="0.45">
+      <c r="B40" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A40" s="8"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A41" s="8" t="s">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B41" s="8"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B42" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A42" s="8"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A43" s="8" t="s">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B43" s="8"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B44" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A44" s="8"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A45" s="8" t="s">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B45" s="8"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B46" s="8" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O2:P20">
-    <sortCondition ref="O6:O20"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="P3:Q21">
+    <sortCondition ref="P7:P21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>